<commit_message>
Edit ATFM aiport file
</commit_message>
<xml_diff>
--- a/static/download/2021/RP3_APT_ATFM_ARR_2021_Jan_Jun.xlsx
+++ b/static/download/2021/RP3_APT_ATFM_ARR_2021_Jan_Jun.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="27" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1370,89 +1370,106 @@
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFF3F3F3"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2182,7 +2199,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="HEGENDORFER Holger" refreshedDate="44390.951248611113" refreshedVersion="6" recordCount="149">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="HEGENDORFER Holger" refreshedDate="44391.373039814818" refreshedVersion="6" recordCount="149">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:F154" sheet="APT_ATFM_APT"/>
   </cacheSource>
@@ -3436,7 +3453,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="APT_ATFM_LOC" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="APT_ATFM_LOC" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="A5:D29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField name="State" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
@@ -3838,7 +3855,9 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3934,13 +3953,13 @@
       </c>
       <c r="B6" s="24">
         <f t="shared" ref="B6:B11" si="0">D6/C6</f>
-        <v>0.55280514839046413</v>
+        <v>0.54943134424648432</v>
       </c>
       <c r="C6" s="25">
-        <v>2410229</v>
+        <v>2455264</v>
       </c>
       <c r="D6" s="25">
-        <v>1332387</v>
+        <v>1348999</v>
       </c>
       <c r="F6" s="19"/>
     </row>
@@ -3950,13 +3969,13 @@
       </c>
       <c r="B7" s="24">
         <f t="shared" si="0"/>
-        <v>0.58681153981254552</v>
+        <v>0.58427588986573298</v>
       </c>
       <c r="C7" s="25">
-        <v>2496713</v>
+        <v>2540608</v>
       </c>
       <c r="D7" s="25">
-        <v>1465100</v>
+        <v>1484416</v>
       </c>
       <c r="F7" s="19"/>
     </row>
@@ -3966,13 +3985,13 @@
       </c>
       <c r="B8" s="24">
         <f t="shared" si="0"/>
-        <v>0.6816868976722168</v>
+        <v>0.67230666889046087</v>
       </c>
       <c r="C8" s="25">
-        <v>2566605</v>
+        <v>2608155</v>
       </c>
       <c r="D8" s="25">
-        <v>1749621</v>
+        <v>1753480</v>
       </c>
       <c r="F8" s="19"/>
     </row>
@@ -3982,13 +4001,13 @@
       </c>
       <c r="B9" s="24">
         <f t="shared" si="0"/>
-        <v>0.84703027793718522</v>
+        <v>0.83517446977400722</v>
       </c>
       <c r="C9" s="25">
-        <v>2627788</v>
+        <v>2675793</v>
       </c>
       <c r="D9" s="25">
-        <v>2225816</v>
+        <v>2234754</v>
       </c>
       <c r="F9" s="19"/>
     </row>
@@ -3998,13 +4017,13 @@
       </c>
       <c r="B10" s="24">
         <f t="shared" si="0"/>
-        <v>0.48255248111514543</v>
+        <v>0.47506053985029995</v>
       </c>
       <c r="C10" s="25">
-        <v>1198050</v>
+        <v>1216967</v>
       </c>
       <c r="D10" s="25">
-        <v>578122</v>
+        <v>578133</v>
       </c>
       <c r="F10" s="19"/>
     </row>
@@ -4173,13 +4192,13 @@
       </c>
       <c r="B6" s="53">
         <f t="shared" ref="B6:B35" si="0">D6/C6</f>
-        <v>0.47353873897874388</v>
+        <v>0.47472769458556535</v>
       </c>
       <c r="C6" s="54">
-        <v>390382</v>
+        <v>397807</v>
       </c>
       <c r="D6" s="55">
-        <v>184861</v>
+        <v>188850</v>
       </c>
       <c r="E6" s="56"/>
       <c r="F6" s="57">
@@ -4193,13 +4212,13 @@
       </c>
       <c r="B7" s="53">
         <f t="shared" si="0"/>
-        <v>0.45454644191502303</v>
+        <v>0.44891574092811726</v>
       </c>
       <c r="C7" s="54">
-        <v>368288</v>
+        <v>375556</v>
       </c>
       <c r="D7" s="55">
-        <v>167404</v>
+        <v>168593</v>
       </c>
       <c r="E7" s="56"/>
       <c r="F7" s="57">
@@ -4213,13 +4232,13 @@
       </c>
       <c r="B8" s="53">
         <f t="shared" si="0"/>
-        <v>1.0336555514043442</v>
+        <v>1.0146129551029313</v>
       </c>
       <c r="C8" s="54">
-        <v>422902</v>
+        <v>430919</v>
       </c>
       <c r="D8" s="55">
-        <v>437135</v>
+        <v>437216</v>
       </c>
       <c r="E8" s="56"/>
       <c r="F8" s="57">
@@ -4233,13 +4252,13 @@
       </c>
       <c r="B9" s="53">
         <f t="shared" si="0"/>
-        <v>0.73711216685316805</v>
+        <v>0.72734085308834739</v>
       </c>
       <c r="C9" s="54">
-        <v>454867</v>
+        <v>463047</v>
       </c>
       <c r="D9" s="55">
-        <v>335288</v>
+        <v>336793</v>
       </c>
       <c r="E9" s="56"/>
       <c r="F9" s="57">
@@ -4253,13 +4272,13 @@
       </c>
       <c r="B10" s="53">
         <f t="shared" si="0"/>
-        <v>1.0639428819188796</v>
+        <v>1.0458497690129751</v>
       </c>
       <c r="C10" s="54">
-        <v>488952</v>
+        <v>497647</v>
       </c>
       <c r="D10" s="55">
-        <v>520217</v>
+        <v>520464</v>
       </c>
       <c r="E10" s="56"/>
       <c r="F10" s="57">
@@ -4273,13 +4292,13 @@
       </c>
       <c r="B11" s="53">
         <f t="shared" si="0"/>
-        <v>1.1562787994355062</v>
+        <v>1.1409917837503449</v>
       </c>
       <c r="C11" s="54">
-        <v>502397</v>
+        <v>510817</v>
       </c>
       <c r="D11" s="55">
-        <v>580911</v>
+        <v>582838</v>
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="57">
@@ -4293,13 +4312,13 @@
       </c>
       <c r="B12" s="53">
         <f t="shared" si="0"/>
-        <v>1.075725456988682</v>
+        <v>1.0594212876744282</v>
       </c>
       <c r="C12" s="54">
-        <v>523153</v>
+        <v>531594</v>
       </c>
       <c r="D12" s="55">
-        <v>562769</v>
+        <v>563182</v>
       </c>
       <c r="E12" s="59" t="s">
         <v>8</v>
@@ -4315,10 +4334,10 @@
       </c>
       <c r="B13" s="53">
         <f t="shared" si="0"/>
-        <v>0.84183939977892774</v>
+        <v>0.82849485345933016</v>
       </c>
       <c r="C13" s="54">
-        <v>511145</v>
+        <v>519378</v>
       </c>
       <c r="D13" s="55">
         <v>430302</v>
@@ -4335,13 +4354,13 @@
       </c>
       <c r="B14" s="53">
         <f t="shared" si="0"/>
-        <v>0.97228430668090526</v>
+        <v>0.95647600647893372</v>
       </c>
       <c r="C14" s="54">
-        <v>503794</v>
+        <v>512430</v>
       </c>
       <c r="D14" s="55">
-        <v>489831</v>
+        <v>490127</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="57">
@@ -4355,13 +4374,13 @@
       </c>
       <c r="B15" s="53">
         <f t="shared" si="0"/>
-        <v>0.79043436789653954</v>
+        <v>0.7815084111694488</v>
       </c>
       <c r="C15" s="54">
-        <v>484359</v>
+        <v>492916</v>
       </c>
       <c r="D15" s="55">
-        <v>382854</v>
+        <v>385218</v>
       </c>
       <c r="E15" s="56"/>
       <c r="F15" s="57">
@@ -4375,13 +4394,13 @@
       </c>
       <c r="B16" s="53">
         <f t="shared" si="0"/>
-        <v>0.44667506278308727</v>
+        <v>0.45141927576821039</v>
       </c>
       <c r="C16" s="54">
-        <v>399391</v>
+        <v>406334</v>
       </c>
       <c r="D16" s="55">
-        <v>178398</v>
+        <v>183427</v>
       </c>
       <c r="E16" s="56"/>
       <c r="F16" s="57">
@@ -4395,13 +4414,13 @@
       </c>
       <c r="B17" s="60">
         <f t="shared" si="0"/>
-        <v>0.73485871512215639</v>
+        <v>0.72485907343114198</v>
       </c>
       <c r="C17" s="61">
-        <v>394699</v>
+        <v>401805</v>
       </c>
       <c r="D17" s="62">
-        <v>290048</v>
+        <v>291252</v>
       </c>
       <c r="E17" s="63"/>
       <c r="F17" s="64">
@@ -4415,17 +4434,17 @@
       </c>
       <c r="B18" s="65">
         <f t="shared" si="0"/>
-        <v>0.612239277698849</v>
+        <v>0.60206824290465122</v>
       </c>
       <c r="C18" s="66">
-        <v>388536</v>
+        <v>395118</v>
       </c>
       <c r="D18" s="67">
-        <v>237877</v>
+        <v>237888</v>
       </c>
       <c r="E18" s="59">
         <f>D18/C18</f>
-        <v>0.612239277698849</v>
+        <v>0.60206824290465122</v>
       </c>
       <c r="F18" s="68">
         <v>1</v>
@@ -4438,17 +4457,17 @@
       </c>
       <c r="B19" s="53">
         <f t="shared" si="0"/>
-        <v>0.69459273036654134</v>
+        <v>0.68288660555493985</v>
       </c>
       <c r="C19" s="54">
-        <v>372591</v>
+        <v>378978</v>
       </c>
       <c r="D19" s="55">
         <v>258799</v>
       </c>
       <c r="E19" s="56">
         <f t="shared" ref="E19:E29" si="1">SUM(D$18:D19)/SUM(C$18:C19)</f>
-        <v>0.65255338465196999</v>
+        <v>0.64163488766251209</v>
       </c>
       <c r="F19" s="57">
         <v>1</v>
@@ -4461,17 +4480,17 @@
       </c>
       <c r="B20" s="53">
         <f t="shared" si="0"/>
-        <v>0.33040598786512382</v>
+        <v>0.32472007592265989</v>
       </c>
       <c r="C20" s="54">
-        <v>241288</v>
+        <v>245513</v>
       </c>
       <c r="D20" s="55">
         <v>79723</v>
       </c>
       <c r="E20" s="56">
         <f t="shared" si="1"/>
-        <v>0.57501035000473855</v>
+        <v>0.56532455088175959</v>
       </c>
       <c r="F20" s="57">
         <v>1</v>
@@ -4484,17 +4503,17 @@
       </c>
       <c r="B21" s="53">
         <f t="shared" si="0"/>
-        <v>2.9030817329164804E-4</v>
+        <v>2.8777615442511181E-4</v>
       </c>
       <c r="C21" s="54">
-        <v>44780</v>
+        <v>45174</v>
       </c>
       <c r="D21" s="54">
         <v>13</v>
       </c>
       <c r="E21" s="56">
         <f t="shared" si="1"/>
-        <v>0.55043425532016477</v>
+        <v>0.54135255728162457</v>
       </c>
       <c r="F21" s="57">
         <v>1</v>
@@ -4507,17 +4526,17 @@
       </c>
       <c r="B22" s="53">
         <f t="shared" si="0"/>
-        <v>7.5806536130373272E-3</v>
+        <v>7.5244022954628204E-3</v>
       </c>
       <c r="C22" s="54">
-        <v>57251</v>
+        <v>57679</v>
       </c>
       <c r="D22" s="54">
         <v>434</v>
       </c>
       <c r="E22" s="56">
         <f t="shared" si="1"/>
-        <v>0.5222944354001916</v>
+        <v>0.51392118396881137</v>
       </c>
       <c r="F22" s="57">
         <v>1</v>
@@ -4530,17 +4549,17 @@
       </c>
       <c r="B23" s="53">
         <f t="shared" si="0"/>
-        <v>1.3631896072817401E-2</v>
+        <v>1.3501931114755833E-2</v>
       </c>
       <c r="C23" s="54">
-        <v>93604</v>
+        <v>94505</v>
       </c>
       <c r="D23" s="54">
         <v>1276</v>
       </c>
       <c r="E23" s="56">
         <f t="shared" si="1"/>
-        <v>0.48255248111514543</v>
+        <v>0.47506053985029995</v>
       </c>
       <c r="F23" s="57">
         <v>1</v>
@@ -4553,17 +4572,17 @@
       </c>
       <c r="B24" s="53">
         <f t="shared" si="0"/>
-        <v>6.548320565704184E-2</v>
+        <v>6.74551731169796E-2</v>
       </c>
       <c r="C24" s="54">
-        <v>203640</v>
+        <v>205959</v>
       </c>
       <c r="D24" s="54">
-        <v>13335</v>
+        <v>13893</v>
       </c>
       <c r="E24" s="56">
         <f t="shared" si="1"/>
-        <v>0.42195991981108522</v>
+        <v>0.41606239537403911</v>
       </c>
       <c r="F24" s="57">
         <v>1</v>
@@ -4576,17 +4595,17 @@
       </c>
       <c r="B25" s="53">
         <f t="shared" si="0"/>
-        <v>6.688313794165815E-2</v>
+        <v>6.691098048964339E-2</v>
       </c>
       <c r="C25" s="54">
-        <v>246684</v>
+        <v>249406</v>
       </c>
       <c r="D25" s="54">
-        <v>16499</v>
+        <v>16688</v>
       </c>
       <c r="E25" s="56">
         <f t="shared" si="1"/>
-        <v>0.36882163877857815</v>
+        <v>0.3639911213802044</v>
       </c>
       <c r="F25" s="57">
         <v>1</v>
@@ -4599,17 +4618,17 @@
       </c>
       <c r="B26" s="53">
         <f t="shared" si="0"/>
-        <v>3.4593277233641424E-2</v>
+        <v>3.4149042891706269E-2</v>
       </c>
       <c r="C26" s="54">
-        <v>217470</v>
+        <v>220299</v>
       </c>
       <c r="D26" s="54">
         <v>7523</v>
       </c>
       <c r="E26" s="56">
         <f t="shared" si="1"/>
-        <v>0.32986626963454607</v>
+        <v>0.32559806956559412</v>
       </c>
       <c r="F26" s="57">
         <v>1</v>
@@ -4622,17 +4641,17 @@
       </c>
       <c r="B27" s="53">
         <f t="shared" si="0"/>
-        <v>4.8599193577833301E-2</v>
+        <v>5.1648334696018386E-2</v>
       </c>
       <c r="C27" s="54">
-        <v>191711</v>
+        <v>194469</v>
       </c>
       <c r="D27" s="54">
-        <v>9317</v>
+        <v>10044</v>
       </c>
       <c r="E27" s="56">
         <f t="shared" si="1"/>
-        <v>0.30365944045238158</v>
+        <v>0.30007234919265968</v>
       </c>
       <c r="F27" s="57">
         <v>1</v>
@@ -4645,17 +4664,17 @@
       </c>
       <c r="B28" s="53">
         <f t="shared" si="0"/>
-        <v>3.183557566738543E-2</v>
+        <v>3.175841488169176E-2</v>
       </c>
       <c r="C28" s="54">
-        <v>131708</v>
+        <v>132028</v>
       </c>
       <c r="D28" s="54">
         <v>4193</v>
       </c>
       <c r="E28" s="56">
         <f t="shared" si="1"/>
-        <v>0.28730627613036896</v>
+        <v>0.2841088932229236</v>
       </c>
       <c r="F28" s="57">
         <v>1</v>
@@ -4678,7 +4697,7 @@
       </c>
       <c r="E29" s="63">
         <f t="shared" si="1"/>
-        <v>0.27184138877421232</v>
+        <v>0.26903355411528068</v>
       </c>
       <c r="F29" s="69">
         <v>1</v>
@@ -5298,7 +5317,7 @@
   <dimension ref="A1:F530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5835,7 +5854,7 @@
         <v>1932</v>
       </c>
       <c r="E29" s="80">
-        <f>D29/C29</f>
+        <f t="shared" si="0"/>
         <v>5.9240180296200901E-2</v>
       </c>
       <c r="F29" s="78"/>

</xml_diff>